<commit_message>
added new sololearn task
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -456,16 +456,21 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is Delhi 
+</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Meron</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>21</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>